<commit_message>
correct a fish species name
</commit_message>
<xml_diff>
--- a/Tables/sampling_summary.xlsx
+++ b/Tables/sampling_summary.xlsx
@@ -890,7 +890,7 @@
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Garra nana</t>
+          <t>Garra jordanica</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -908,8 +908,8 @@
       <c r="G9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>0</v>
+      <c r="H9" s="12" t="n">
+        <v>1</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>0</v>
@@ -920,14 +920,14 @@
       <c r="K9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2" t="n">
-        <v>0</v>
+      <c r="L9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="N9" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>0</v>
@@ -946,7 +946,7 @@
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Garra rufa</t>
+          <t>Garra nana</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -964,26 +964,26 @@
       <c r="G10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="12" t="n">
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="N10" s="10" t="n">
-        <v>5</v>
+      <c r="M10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>0</v>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Mugil liza</t>
+          <t>Mugil</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>OH</t>
+          <t>Coptodon zillii</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1379,17 +1379,17 @@
       <c r="H17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <v>0</v>
+      <c r="I17" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="J17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="n">
-        <v>0</v>
+      <c r="K17" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L17" s="3" t="n">
+        <v>4</v>
       </c>
       <c r="M17" s="2" t="n">
         <v>0</v>
@@ -1400,21 +1400,21 @@
       <c r="O17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P17" s="7" t="n">
-        <v>1</v>
+      <c r="P17" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="Q17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="R17" s="13" t="n">
-        <v>4</v>
+      <c r="R17" s="8" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Oreochromis aureus</t>
+          <t>OH</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1435,42 +1435,42 @@
       <c r="H18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" s="13" t="n">
         <v>4</v>
-      </c>
-      <c r="J18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" s="2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Sarotherodon  galilaeus</t>
+          <t>Oreochromis aureus</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1491,14 +1491,14 @@
       <c r="H19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="2" t="n">
-        <v>0</v>
+      <c r="I19" s="3" t="n">
+        <v>4</v>
       </c>
       <c r="J19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K19" s="15" t="n">
-        <v>3</v>
+      <c r="K19" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="L19" s="2" t="n">
         <v>0</v>
@@ -1512,21 +1512,21 @@
       <c r="O19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P19" s="13" t="n">
-        <v>4</v>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="Q19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="R19" s="13" t="n">
-        <v>4</v>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Tilapia zillii</t>
+          <t>Sarotherodon  galilaeus</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1547,35 +1547,35 @@
       <c r="H20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="4" t="n">
-        <v>1</v>
+      <c r="I20" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="J20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K20" s="3" t="n">
+      <c r="K20" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="Q20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="13" t="n">
         <v>4</v>
-      </c>
-      <c r="M20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" s="8" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>